<commit_message>
use Axisapp_web.py with axis_pro_gf.xlsx
</commit_message>
<xml_diff>
--- a/axis_pro_gf.xlsx
+++ b/axis_pro_gf.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gulmira/Documents/Axis web/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11AC5C75-6A7D-F745-B538-04875B885407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F077709-A1B8-2B41-B2A2-6CD76EC25131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="СПРАВОЧНИК -1" sheetId="1" r:id="rId1"/>
     <sheet name="СПРАВОЧНИК -2" sheetId="2" r:id="rId2"/>
-    <sheet name="ПОЛЬЗОВАТЕЛИ" sheetId="8" r:id="rId3"/>
-    <sheet name="СПРАВОЧНИК -3" sheetId="3" r:id="rId4"/>
+    <sheet name="СПРАВОЧНИК -3" sheetId="3" r:id="rId3"/>
+    <sheet name="ПОЛЬЗОВАТЕЛИ" sheetId="8" r:id="rId4"/>
     <sheet name="ЗАПРОСЫ" sheetId="4" r:id="rId5"/>
     <sheet name="Расчет по габаритам" sheetId="5" r:id="rId6"/>
     <sheet name="Расчетом расходов материалов" sheetId="6" r:id="rId7"/>
@@ -1979,14 +1979,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Y853"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomLeft" activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2001,7 +2001,7 @@
     <col min="15" max="15" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15.75" customHeight="1">
+    <row r="1" spans="1:25" ht="40" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="15.75" hidden="1" customHeight="1">
+    <row r="7" spans="1:25" ht="15.75" customHeight="1">
       <c r="A7" s="7" t="s">
         <v>15</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="15.75" hidden="1" customHeight="1">
+    <row r="8" spans="1:25" ht="15.75" customHeight="1">
       <c r="A8" s="7" t="s">
         <v>15</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="15.75" hidden="1" customHeight="1">
+    <row r="9" spans="1:25" ht="15.75" customHeight="1">
       <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
@@ -2410,7 +2410,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="15.75" hidden="1" customHeight="1">
+    <row r="10" spans="1:25" ht="15.75" customHeight="1">
       <c r="A10" s="7" t="s">
         <v>15</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="15.75" hidden="1" customHeight="1">
+    <row r="11" spans="1:25" ht="15.75" customHeight="1">
       <c r="A11" s="7" t="s">
         <v>15</v>
       </c>
@@ -2498,7 +2498,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="15.75" hidden="1" customHeight="1">
+    <row r="12" spans="1:25" ht="15.75" customHeight="1">
       <c r="A12" s="7" t="s">
         <v>15</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="15.75" hidden="1" customHeight="1">
+    <row r="13" spans="1:25" ht="15.75" customHeight="1">
       <c r="A13" s="7" t="s">
         <v>15</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="15.75" hidden="1" customHeight="1">
+    <row r="14" spans="1:25" ht="15.75" customHeight="1">
       <c r="A14" s="7" t="s">
         <v>15</v>
       </c>
@@ -2630,7 +2630,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="15.75" hidden="1" customHeight="1">
+    <row r="15" spans="1:25" ht="15.75" customHeight="1">
       <c r="A15" s="7" t="s">
         <v>15</v>
       </c>
@@ -2895,7 +2895,7 @@
       </c>
       <c r="P20" s="12"/>
     </row>
-    <row r="21" spans="1:20" ht="15.75" hidden="1" customHeight="1">
+    <row r="21" spans="1:20" ht="15.75" customHeight="1">
       <c r="A21" s="7" t="s">
         <v>103</v>
       </c>
@@ -2940,7 +2940,7 @@
       </c>
       <c r="P21" s="12"/>
     </row>
-    <row r="22" spans="1:20" ht="15.75" hidden="1" customHeight="1">
+    <row r="22" spans="1:20" ht="15.75" customHeight="1">
       <c r="A22" s="7" t="s">
         <v>103</v>
       </c>
@@ -2985,7 +2985,7 @@
       </c>
       <c r="P22" s="12"/>
     </row>
-    <row r="23" spans="1:20" ht="15.75" hidden="1" customHeight="1">
+    <row r="23" spans="1:20" ht="15.75" customHeight="1">
       <c r="A23" s="7" t="s">
         <v>103</v>
       </c>
@@ -3030,7 +3030,7 @@
       </c>
       <c r="P23" s="12"/>
     </row>
-    <row r="24" spans="1:20" ht="15.75" hidden="1" customHeight="1">
+    <row r="24" spans="1:20" ht="15.75" customHeight="1">
       <c r="A24" s="7" t="s">
         <v>103</v>
       </c>
@@ -3222,7 +3222,7 @@
       <c r="S27" s="12"/>
       <c r="T27" s="12"/>
     </row>
-    <row r="28" spans="1:20" ht="15.75" hidden="1" customHeight="1">
+    <row r="28" spans="1:20" ht="15.75" customHeight="1">
       <c r="A28" s="7" t="s">
         <v>15</v>
       </c>
@@ -3271,7 +3271,7 @@
       <c r="S28" s="12"/>
       <c r="T28" s="12"/>
     </row>
-    <row r="29" spans="1:20" ht="15.75" hidden="1" customHeight="1">
+    <row r="29" spans="1:20" ht="15.75" customHeight="1">
       <c r="A29" s="7" t="s">
         <v>15</v>
       </c>
@@ -3320,7 +3320,7 @@
       <c r="S29" s="12"/>
       <c r="T29" s="12"/>
     </row>
-    <row r="30" spans="1:20" ht="15.75" hidden="1" customHeight="1">
+    <row r="30" spans="1:20" ht="15.75" customHeight="1">
       <c r="A30" s="7" t="s">
         <v>15</v>
       </c>
@@ -3369,7 +3369,7 @@
       <c r="S30" s="12"/>
       <c r="T30" s="12"/>
     </row>
-    <row r="31" spans="1:20" ht="15.75" hidden="1" customHeight="1">
+    <row r="31" spans="1:20" ht="15.75" customHeight="1">
       <c r="A31" s="7" t="s">
         <v>15</v>
       </c>
@@ -3418,7 +3418,7 @@
       <c r="S31" s="12"/>
       <c r="T31" s="12"/>
     </row>
-    <row r="32" spans="1:20" ht="15.75" hidden="1" customHeight="1">
+    <row r="32" spans="1:20" ht="15.75" customHeight="1">
       <c r="A32" s="7" t="s">
         <v>15</v>
       </c>
@@ -3467,7 +3467,7 @@
       <c r="S32" s="12"/>
       <c r="T32" s="12"/>
     </row>
-    <row r="33" spans="1:20" ht="15.75" hidden="1" customHeight="1">
+    <row r="33" spans="1:20" ht="15.75" customHeight="1">
       <c r="A33" s="7" t="s">
         <v>15</v>
       </c>
@@ -3516,7 +3516,7 @@
       <c r="S33" s="12"/>
       <c r="T33" s="12"/>
     </row>
-    <row r="34" spans="1:20" ht="15.75" hidden="1" customHeight="1">
+    <row r="34" spans="1:20" ht="15.75" customHeight="1">
       <c r="A34" s="7" t="s">
         <v>15</v>
       </c>
@@ -3908,7 +3908,7 @@
       <c r="S41" s="12"/>
       <c r="T41" s="12"/>
     </row>
-    <row r="42" spans="1:20" ht="15.75" hidden="1" customHeight="1">
+    <row r="42" spans="1:20" ht="15.75" customHeight="1">
       <c r="A42" s="7" t="s">
         <v>103</v>
       </c>
@@ -4202,7 +4202,7 @@
       <c r="S47" s="12"/>
       <c r="T47" s="12"/>
     </row>
-    <row r="48" spans="1:20" ht="15.75" hidden="1" customHeight="1">
+    <row r="48" spans="1:20" ht="15.75" customHeight="1">
       <c r="A48" s="7" t="s">
         <v>103</v>
       </c>
@@ -4251,7 +4251,7 @@
       <c r="S48" s="12"/>
       <c r="T48" s="12"/>
     </row>
-    <row r="49" spans="1:20" ht="15.75" hidden="1" customHeight="1">
+    <row r="49" spans="1:20" ht="15.75" customHeight="1">
       <c r="A49" s="7" t="s">
         <v>103</v>
       </c>
@@ -4300,7 +4300,7 @@
       <c r="S49" s="12"/>
       <c r="T49" s="12"/>
     </row>
-    <row r="50" spans="1:20" ht="15.75" hidden="1" customHeight="1">
+    <row r="50" spans="1:20" ht="15.75" customHeight="1">
       <c r="A50" s="7" t="s">
         <v>103</v>
       </c>
@@ -4349,7 +4349,7 @@
       <c r="S50" s="6"/>
       <c r="T50" s="6"/>
     </row>
-    <row r="51" spans="1:20" ht="15.75" hidden="1" customHeight="1">
+    <row r="51" spans="1:20" ht="15.75" customHeight="1">
       <c r="A51" s="7" t="s">
         <v>103</v>
       </c>
@@ -4643,7 +4643,7 @@
       <c r="S56" s="12"/>
       <c r="T56" s="12"/>
     </row>
-    <row r="57" spans="1:20" ht="13" hidden="1" customHeight="1">
+    <row r="57" spans="1:20" ht="13" customHeight="1">
       <c r="A57" s="7" t="s">
         <v>103</v>
       </c>
@@ -4839,7 +4839,7 @@
       <c r="S60" s="12"/>
       <c r="T60" s="12"/>
     </row>
-    <row r="61" spans="1:20" ht="13" hidden="1" customHeight="1">
+    <row r="61" spans="1:20" ht="13" customHeight="1">
       <c r="A61" s="7" t="s">
         <v>103</v>
       </c>
@@ -4888,7 +4888,7 @@
       <c r="S61" s="12"/>
       <c r="T61" s="12"/>
     </row>
-    <row r="62" spans="1:20" ht="13" hidden="1" customHeight="1">
+    <row r="62" spans="1:20" ht="13" customHeight="1">
       <c r="A62" s="7" t="s">
         <v>103</v>
       </c>
@@ -4937,7 +4937,7 @@
       <c r="S62" s="12"/>
       <c r="T62" s="12"/>
     </row>
-    <row r="63" spans="1:20" ht="13" hidden="1" customHeight="1">
+    <row r="63" spans="1:20" ht="13" customHeight="1">
       <c r="A63" s="7" t="s">
         <v>103</v>
       </c>
@@ -4986,7 +4986,7 @@
       <c r="S63" s="12"/>
       <c r="T63" s="12"/>
     </row>
-    <row r="64" spans="1:20" ht="13" hidden="1" customHeight="1">
+    <row r="64" spans="1:20" ht="13" customHeight="1">
       <c r="A64" s="7" t="s">
         <v>103</v>
       </c>
@@ -5035,7 +5035,7 @@
       <c r="S64" s="12"/>
       <c r="T64" s="12"/>
     </row>
-    <row r="65" spans="1:20" ht="13" hidden="1" customHeight="1">
+    <row r="65" spans="1:20" ht="13" customHeight="1">
       <c r="A65" s="7" t="s">
         <v>103</v>
       </c>
@@ -5084,7 +5084,7 @@
       <c r="S65" s="12"/>
       <c r="T65" s="12"/>
     </row>
-    <row r="66" spans="1:20" ht="13" hidden="1" customHeight="1">
+    <row r="66" spans="1:20" ht="13" customHeight="1">
       <c r="A66" s="7" t="s">
         <v>103</v>
       </c>
@@ -5133,7 +5133,7 @@
       <c r="S66" s="12"/>
       <c r="T66" s="12"/>
     </row>
-    <row r="67" spans="1:20" ht="13" hidden="1" customHeight="1">
+    <row r="67" spans="1:20" ht="13" customHeight="1">
       <c r="A67" s="7" t="s">
         <v>103</v>
       </c>
@@ -5182,7 +5182,7 @@
       <c r="S67" s="12"/>
       <c r="T67" s="12"/>
     </row>
-    <row r="68" spans="1:20" ht="13" hidden="1" customHeight="1">
+    <row r="68" spans="1:20" ht="13" customHeight="1">
       <c r="A68" s="7" t="s">
         <v>103</v>
       </c>
@@ -5476,7 +5476,7 @@
       <c r="S73" s="12"/>
       <c r="T73" s="12"/>
     </row>
-    <row r="74" spans="1:20" ht="13" hidden="1" customHeight="1">
+    <row r="74" spans="1:20" ht="13" customHeight="1">
       <c r="A74" s="7" t="s">
         <v>103</v>
       </c>
@@ -5525,7 +5525,7 @@
       <c r="S74" s="6"/>
       <c r="T74" s="6"/>
     </row>
-    <row r="75" spans="1:20" ht="13" hidden="1" customHeight="1">
+    <row r="75" spans="1:20" ht="13" customHeight="1">
       <c r="A75" s="7" t="s">
         <v>103</v>
       </c>
@@ -5574,7 +5574,7 @@
       <c r="S75" s="12"/>
       <c r="T75" s="12"/>
     </row>
-    <row r="76" spans="1:20" ht="13" hidden="1" customHeight="1">
+    <row r="76" spans="1:20" ht="13" customHeight="1">
       <c r="A76" s="7" t="s">
         <v>103</v>
       </c>
@@ -5623,7 +5623,7 @@
       <c r="S76" s="12"/>
       <c r="T76" s="12"/>
     </row>
-    <row r="77" spans="1:20" ht="13" hidden="1" customHeight="1">
+    <row r="77" spans="1:20" ht="13" customHeight="1">
       <c r="A77" s="7" t="s">
         <v>103</v>
       </c>
@@ -5868,7 +5868,7 @@
       <c r="S81" s="12"/>
       <c r="T81" s="12"/>
     </row>
-    <row r="82" spans="1:20" ht="13" hidden="1" customHeight="1">
+    <row r="82" spans="1:20" ht="13" customHeight="1">
       <c r="A82" s="7" t="s">
         <v>103</v>
       </c>
@@ -5917,7 +5917,7 @@
       <c r="S82" s="12"/>
       <c r="T82" s="12"/>
     </row>
-    <row r="83" spans="1:20" ht="13" hidden="1" customHeight="1">
+    <row r="83" spans="1:20" ht="13" customHeight="1">
       <c r="A83" s="7" t="s">
         <v>103</v>
       </c>
@@ -5966,7 +5966,7 @@
       <c r="S83" s="12"/>
       <c r="T83" s="12"/>
     </row>
-    <row r="84" spans="1:20" ht="13" hidden="1" customHeight="1">
+    <row r="84" spans="1:20" ht="13" customHeight="1">
       <c r="A84" s="7" t="s">
         <v>103</v>
       </c>
@@ -6211,7 +6211,7 @@
       <c r="S88" s="12"/>
       <c r="T88" s="12"/>
     </row>
-    <row r="89" spans="1:20" ht="13" hidden="1" customHeight="1">
+    <row r="89" spans="1:20" ht="13" customHeight="1">
       <c r="A89" s="7" t="s">
         <v>103</v>
       </c>
@@ -6260,7 +6260,7 @@
       <c r="S89" s="12"/>
       <c r="T89" s="12"/>
     </row>
-    <row r="90" spans="1:20" ht="13" hidden="1" customHeight="1">
+    <row r="90" spans="1:20" ht="13" customHeight="1">
       <c r="A90" s="7" t="s">
         <v>103</v>
       </c>
@@ -6309,7 +6309,7 @@
       <c r="S90" s="12"/>
       <c r="T90" s="12"/>
     </row>
-    <row r="91" spans="1:20" ht="13" hidden="1" customHeight="1">
+    <row r="91" spans="1:20" ht="13" customHeight="1">
       <c r="A91" s="7" t="s">
         <v>103</v>
       </c>
@@ -6358,7 +6358,7 @@
       <c r="S91" s="12"/>
       <c r="T91" s="12"/>
     </row>
-    <row r="92" spans="1:20" ht="13" hidden="1" customHeight="1">
+    <row r="92" spans="1:20" ht="13" customHeight="1">
       <c r="A92" s="7" t="s">
         <v>103</v>
       </c>
@@ -6407,7 +6407,7 @@
       <c r="S92" s="12"/>
       <c r="T92" s="12"/>
     </row>
-    <row r="93" spans="1:20" ht="13" hidden="1" customHeight="1">
+    <row r="93" spans="1:20" ht="13" customHeight="1">
       <c r="A93" s="7" t="s">
         <v>103</v>
       </c>
@@ -6456,7 +6456,7 @@
       <c r="S93" s="12"/>
       <c r="T93" s="12"/>
     </row>
-    <row r="94" spans="1:20" ht="13" hidden="1" customHeight="1">
+    <row r="94" spans="1:20" ht="13" customHeight="1">
       <c r="A94" s="7" t="s">
         <v>103</v>
       </c>
@@ -6505,7 +6505,7 @@
       <c r="S94" s="12"/>
       <c r="T94" s="12"/>
     </row>
-    <row r="95" spans="1:20" ht="13" hidden="1" customHeight="1">
+    <row r="95" spans="1:20" ht="13" customHeight="1">
       <c r="A95" s="7" t="s">
         <v>103</v>
       </c>
@@ -6554,7 +6554,7 @@
       <c r="S95" s="12"/>
       <c r="T95" s="12"/>
     </row>
-    <row r="96" spans="1:20" ht="13" hidden="1" customHeight="1">
+    <row r="96" spans="1:20" ht="13" customHeight="1">
       <c r="A96" s="7" t="s">
         <v>103</v>
       </c>
@@ -6603,7 +6603,7 @@
       <c r="S96" s="12"/>
       <c r="T96" s="12"/>
     </row>
-    <row r="97" spans="1:21" ht="13" hidden="1" customHeight="1">
+    <row r="97" spans="1:21" ht="13" customHeight="1">
       <c r="A97" s="7" t="s">
         <v>103</v>
       </c>
@@ -6898,7 +6898,7 @@
       <c r="T102" s="12"/>
       <c r="U102" s="12"/>
     </row>
-    <row r="103" spans="1:21" ht="13" hidden="1" customHeight="1">
+    <row r="103" spans="1:21" ht="13" customHeight="1">
       <c r="A103" s="7" t="s">
         <v>103</v>
       </c>
@@ -7145,7 +7145,7 @@
       <c r="T107" s="12"/>
       <c r="U107" s="12"/>
     </row>
-    <row r="108" spans="1:21" ht="13" hidden="1" customHeight="1">
+    <row r="108" spans="1:21" ht="13" customHeight="1">
       <c r="A108" s="7" t="s">
         <v>103</v>
       </c>
@@ -7195,7 +7195,7 @@
       <c r="T108" s="12"/>
       <c r="U108" s="12"/>
     </row>
-    <row r="109" spans="1:21" ht="13" hidden="1" customHeight="1">
+    <row r="109" spans="1:21" ht="13" customHeight="1">
       <c r="A109" s="7" t="s">
         <v>103</v>
       </c>
@@ -7245,7 +7245,7 @@
       <c r="T109" s="12"/>
       <c r="U109" s="12"/>
     </row>
-    <row r="110" spans="1:21" ht="13" hidden="1" customHeight="1">
+    <row r="110" spans="1:21" ht="13" customHeight="1">
       <c r="A110" s="7" t="s">
         <v>103</v>
       </c>
@@ -7295,7 +7295,7 @@
       <c r="T110" s="12"/>
       <c r="U110" s="12"/>
     </row>
-    <row r="111" spans="1:21" ht="13" hidden="1" customHeight="1">
+    <row r="111" spans="1:21" ht="13" customHeight="1">
       <c r="A111" s="7" t="s">
         <v>103</v>
       </c>
@@ -7345,7 +7345,7 @@
       <c r="T111" s="12"/>
       <c r="U111" s="12"/>
     </row>
-    <row r="112" spans="1:21" ht="13" hidden="1" customHeight="1">
+    <row r="112" spans="1:21" ht="13" customHeight="1">
       <c r="A112" s="7" t="s">
         <v>103</v>
       </c>
@@ -7395,7 +7395,7 @@
       <c r="T112" s="12"/>
       <c r="U112" s="12"/>
     </row>
-    <row r="113" spans="1:21" ht="13" hidden="1" customHeight="1">
+    <row r="113" spans="1:21" ht="13" customHeight="1">
       <c r="A113" s="7" t="s">
         <v>103</v>
       </c>
@@ -7445,7 +7445,7 @@
       <c r="T113" s="12"/>
       <c r="U113" s="12"/>
     </row>
-    <row r="114" spans="1:21" ht="13" hidden="1" customHeight="1">
+    <row r="114" spans="1:21" ht="13" customHeight="1">
       <c r="A114" s="7" t="s">
         <v>103</v>
       </c>
@@ -7495,7 +7495,7 @@
       <c r="T114" s="12"/>
       <c r="U114" s="12"/>
     </row>
-    <row r="115" spans="1:21" ht="13" hidden="1" customHeight="1">
+    <row r="115" spans="1:21" ht="13" customHeight="1">
       <c r="A115" s="7" t="s">
         <v>103</v>
       </c>
@@ -7545,7 +7545,7 @@
       <c r="T115" s="12"/>
       <c r="U115" s="12"/>
     </row>
-    <row r="116" spans="1:21" ht="13" hidden="1" customHeight="1">
+    <row r="116" spans="1:21" ht="13" customHeight="1">
       <c r="A116" s="7" t="s">
         <v>103</v>
       </c>
@@ -7595,7 +7595,7 @@
       <c r="T116" s="12"/>
       <c r="U116" s="12"/>
     </row>
-    <row r="117" spans="1:21" ht="13" hidden="1" customHeight="1">
+    <row r="117" spans="1:21" ht="13" customHeight="1">
       <c r="A117" s="7" t="s">
         <v>103</v>
       </c>
@@ -7645,7 +7645,7 @@
       <c r="T117" s="12"/>
       <c r="U117" s="12"/>
     </row>
-    <row r="118" spans="1:21" ht="13" hidden="1" customHeight="1">
+    <row r="118" spans="1:21" ht="13" customHeight="1">
       <c r="A118" s="7" t="s">
         <v>103</v>
       </c>
@@ -7689,7 +7689,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="119" spans="1:21" ht="13" hidden="1" customHeight="1">
+    <row r="119" spans="1:21" ht="13" customHeight="1">
       <c r="A119" s="7" t="s">
         <v>103</v>
       </c>
@@ -7733,7 +7733,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="120" spans="1:21" ht="13" hidden="1" customHeight="1">
+    <row r="120" spans="1:21" ht="13" customHeight="1">
       <c r="A120" s="7" t="s">
         <v>103</v>
       </c>
@@ -12186,13 +12186,6 @@
       <c r="N853" s="15"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Y120" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="м"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -12205,7 +12198,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -12355,130 +12348,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4EC6FB2-1903-0042-ACE8-47D7240CC83A}">
-  <dimension ref="A1:G47"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
-  <cols>
-    <col min="1" max="1" width="24.83203125" customWidth="1"/>
-    <col min="2" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="25" t="s">
-        <v>503</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>504</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="16">
-      <c r="A2" s="26" t="s">
-        <v>508</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>511</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="16">
-      <c r="A3" s="27" t="s">
-        <v>510</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>509</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="16">
-      <c r="A4" s="28" t="s">
-        <v>512</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>513</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="16">
-      <c r="A5" s="27" t="s">
-        <v>514</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>515</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="16">
-      <c r="A6" s="27" t="s">
-        <v>516</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>517</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="16">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-    </row>
-    <row r="8" spans="1:3" ht="16">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-    </row>
-    <row r="9" spans="1:3" ht="16">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-    </row>
-    <row r="10" spans="1:3" ht="16">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-    </row>
-    <row r="11" spans="1:3" ht="16">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-    </row>
-    <row r="47" spans="7:7">
-      <c r="G47" s="12"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" xr:uid="{BF75923F-2700-EA40-8D2C-95CD49C77160}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -40644,6 +40520,123 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4EC6FB2-1903-0042-ACE8-47D7240CC83A}">
+  <dimension ref="A1:G47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="24.83203125" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="25" t="s">
+        <v>503</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>504</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="16">
+      <c r="A2" s="26" t="s">
+        <v>508</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>511</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16">
+      <c r="A3" s="27" t="s">
+        <v>510</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>509</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16">
+      <c r="A4" s="28" t="s">
+        <v>512</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>513</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16">
+      <c r="A5" s="27" t="s">
+        <v>514</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>515</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16">
+      <c r="A6" s="27" t="s">
+        <v>516</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>517</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+    </row>
+    <row r="8" spans="1:3" ht="16">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+    </row>
+    <row r="9" spans="1:3" ht="16">
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+    </row>
+    <row r="10" spans="1:3" ht="16">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+    </row>
+    <row r="11" spans="1:3" ht="16">
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+    </row>
+    <row r="47" spans="7:7">
+      <c r="G47" s="12"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{BF75923F-2700-EA40-8D2C-95CD49C77160}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:V10"/>

</xml_diff>

<commit_message>
fix(calc): normalize ref2; lambris grouping; tambur details; handles per sash; safe parsing
</commit_message>
<xml_diff>
--- a/axis_pro_gf.xlsx
+++ b/axis_pro_gf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gulmira/Documents/Axis web/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ADBA6866-7372-EF4E-86C3-926052CD8626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56EDC7B8-6D54-5742-B97F-0C1D6E2E13F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="29400" windowHeight="17160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="29400" windowHeight="17160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="СПРАВОЧНИК -1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2846" uniqueCount="712">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2840" uniqueCount="710">
   <si>
     <t>Тип изделия:</t>
   </si>
@@ -2072,12 +2072,6 @@
     <t>Стоимость за шт доводчика</t>
   </si>
   <si>
-    <t>Сэндвич</t>
-  </si>
-  <si>
-    <t>Ламбри</t>
-  </si>
-  <si>
     <t>sum([2*door_height[i]/1000 for i in range(door_count)])</t>
   </si>
   <si>
@@ -2153,18 +2147,12 @@
     <t>Новая Формула_Python</t>
   </si>
   <si>
-    <t xml:space="preserve">Стоимость заполнения </t>
-  </si>
-  <si>
     <t>Ламбри без термо</t>
   </si>
   <si>
     <t>Ламбри с термо</t>
   </si>
   <si>
-    <t>НЕТ</t>
-  </si>
-  <si>
     <t>QWER2020</t>
   </si>
   <si>
@@ -2178,6 +2166,12 @@
   </si>
   <si>
     <t>Qwer234</t>
+  </si>
+  <si>
+    <t>Панели</t>
+  </si>
+  <si>
+    <t>Стоимость Панелей за 1 м в 6 м хлысте</t>
   </si>
 </sst>
 </file>
@@ -10011,7 +10005,7 @@
         <v>0</v>
       </c>
       <c r="O148" s="11" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="Q148" s="11"/>
       <c r="R148" s="11"/>
@@ -10066,7 +10060,7 @@
         <v>0</v>
       </c>
       <c r="O149" s="11" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="Q149" s="11"/>
       <c r="R149" s="11"/>
@@ -10121,7 +10115,7 @@
         <v>0</v>
       </c>
       <c r="O150" s="11" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="Q150" s="11"/>
       <c r="R150" s="11"/>
@@ -10176,7 +10170,7 @@
         <v>0</v>
       </c>
       <c r="O151" s="11" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="Q151" s="11"/>
       <c r="R151" s="11"/>
@@ -10231,7 +10225,7 @@
         <v>0</v>
       </c>
       <c r="O152" s="11" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="Q152" s="11"/>
       <c r="R152" s="11"/>
@@ -10286,7 +10280,7 @@
         <v>0</v>
       </c>
       <c r="O153" s="11" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="Q153" s="11"/>
       <c r="R153" s="11"/>
@@ -10341,7 +10335,7 @@
         <v>0</v>
       </c>
       <c r="O154" s="11" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="Q154" s="11"/>
       <c r="R154" s="11"/>
@@ -10396,7 +10390,7 @@
         <v>0</v>
       </c>
       <c r="O155" s="11" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="Q155" s="11"/>
       <c r="R155" s="11"/>
@@ -10451,7 +10445,7 @@
         <v>0</v>
       </c>
       <c r="O156" s="11" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="Q156" s="11"/>
       <c r="R156" s="11"/>
@@ -10506,7 +10500,7 @@
         <v>0</v>
       </c>
       <c r="O157" s="11" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="Q157" s="11"/>
       <c r="R157" s="11"/>
@@ -10561,7 +10555,7 @@
         <v>0</v>
       </c>
       <c r="O158" s="11" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="Q158" s="11"/>
       <c r="R158" s="11"/>
@@ -10616,7 +10610,7 @@
         <v>0</v>
       </c>
       <c r="O159" s="11" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="Q159" s="11"/>
       <c r="R159" s="11"/>
@@ -10671,7 +10665,7 @@
         <v>0</v>
       </c>
       <c r="O160" s="11" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="Q160" s="11"/>
       <c r="R160" s="11"/>
@@ -10726,7 +10720,7 @@
         <v>0</v>
       </c>
       <c r="O161" s="11" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="Q161" s="11"/>
       <c r="R161" s="11"/>
@@ -10781,7 +10775,7 @@
         <v>0</v>
       </c>
       <c r="O162" s="11" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="Q162" s="11"/>
       <c r="R162" s="11"/>
@@ -10811,7 +10805,7 @@
         <v>197</v>
       </c>
       <c r="F163" s="11" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="G163" s="31" t="s">
         <v>48</v>
@@ -10866,7 +10860,7 @@
         <v>199</v>
       </c>
       <c r="F164" s="11" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="G164" s="31" t="s">
         <v>48</v>
@@ -10921,7 +10915,7 @@
         <v>486</v>
       </c>
       <c r="F165" s="11" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="G165" s="31" t="s">
         <v>21</v>
@@ -10976,7 +10970,7 @@
         <v>224</v>
       </c>
       <c r="F166" s="11" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="G166" s="31" t="s">
         <v>21</v>
@@ -11031,7 +11025,7 @@
         <v>203</v>
       </c>
       <c r="F167" s="11" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="G167" s="31" t="s">
         <v>21</v>
@@ -11086,7 +11080,7 @@
         <v>90</v>
       </c>
       <c r="F168" s="11" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="G168" s="31" t="s">
         <v>21</v>
@@ -11141,7 +11135,7 @@
         <v>98</v>
       </c>
       <c r="F169" s="11" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="G169" s="31" t="s">
         <v>21</v>
@@ -11196,7 +11190,7 @@
         <v>304</v>
       </c>
       <c r="F170" s="11" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="G170" s="31" t="s">
         <v>48</v>
@@ -11251,7 +11245,7 @@
         <v>111</v>
       </c>
       <c r="F171" s="11" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="G171" s="31" t="s">
         <v>48</v>
@@ -11306,7 +11300,7 @@
         <v>269</v>
       </c>
       <c r="F172" s="11" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="G172" s="31" t="s">
         <v>48</v>
@@ -11361,7 +11355,7 @@
         <v>118</v>
       </c>
       <c r="F173" s="11" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="G173" s="31" t="s">
         <v>119</v>
@@ -11416,7 +11410,7 @@
         <v>247</v>
       </c>
       <c r="F174" s="11" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="G174" s="31" t="s">
         <v>119</v>
@@ -11471,7 +11465,7 @@
         <v>313</v>
       </c>
       <c r="F175" s="11" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="G175" s="31" t="s">
         <v>48</v>
@@ -11526,7 +11520,7 @@
         <v>515</v>
       </c>
       <c r="F176" s="11" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="G176" s="31" t="s">
         <v>119</v>
@@ -11581,7 +11575,7 @@
         <v>519</v>
       </c>
       <c r="F177" s="11" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="G177" s="31" t="s">
         <v>499</v>
@@ -11636,7 +11630,7 @@
         <v>523</v>
       </c>
       <c r="F178" s="11" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="G178" s="31" t="s">
         <v>21</v>
@@ -11691,7 +11685,7 @@
         <v>153</v>
       </c>
       <c r="F179" s="11" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="G179" s="31" t="s">
         <v>21</v>
@@ -11746,7 +11740,7 @@
         <v>157</v>
       </c>
       <c r="F180" s="11" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="G180" s="31" t="s">
         <v>21</v>
@@ -11801,7 +11795,7 @@
         <v>160</v>
       </c>
       <c r="F181" s="11" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="G181" s="31" t="s">
         <v>21</v>
@@ -11856,7 +11850,7 @@
         <v>26</v>
       </c>
       <c r="F182" s="11" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="G182" s="31" t="s">
         <v>21</v>
@@ -11911,7 +11905,7 @@
         <v>31</v>
       </c>
       <c r="F183" s="11" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="G183" s="31" t="s">
         <v>21</v>
@@ -11966,7 +11960,7 @@
         <v>41</v>
       </c>
       <c r="F184" s="11" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="G184" s="31" t="s">
         <v>21</v>
@@ -12021,7 +12015,7 @@
         <v>216</v>
       </c>
       <c r="F185" s="11" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="G185" s="31" t="s">
         <v>21</v>
@@ -12076,7 +12070,7 @@
         <v>53</v>
       </c>
       <c r="F186" s="11" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="G186" s="31" t="s">
         <v>48</v>
@@ -12186,7 +12180,7 @@
         <v>338</v>
       </c>
       <c r="F188" s="11" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="G188" s="31" t="s">
         <v>48</v>
@@ -12241,7 +12235,7 @@
         <v>63</v>
       </c>
       <c r="F189" s="11" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="G189" s="31" t="s">
         <v>48</v>
@@ -12351,7 +12345,7 @@
         <v>224</v>
       </c>
       <c r="F191" s="11" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="G191" s="31" t="s">
         <v>21</v>
@@ -12406,7 +12400,7 @@
         <v>94</v>
       </c>
       <c r="F192" s="11" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="G192" s="31" t="s">
         <v>21</v>
@@ -12461,7 +12455,7 @@
         <v>98</v>
       </c>
       <c r="F193" s="11" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="G193" s="31" t="s">
         <v>21</v>
@@ -12516,7 +12510,7 @@
         <v>557</v>
       </c>
       <c r="F194" s="11" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="G194" s="31" t="s">
         <v>48</v>
@@ -12571,7 +12565,7 @@
         <v>237</v>
       </c>
       <c r="F195" s="11" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="G195" s="31" t="s">
         <v>48</v>
@@ -12626,7 +12620,7 @@
         <v>241</v>
       </c>
       <c r="F196" s="11" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="G196" s="31" t="s">
         <v>48</v>
@@ -12681,7 +12675,7 @@
         <v>244</v>
       </c>
       <c r="F197" s="11" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="G197" s="31" t="s">
         <v>48</v>
@@ -12736,7 +12730,7 @@
         <v>567</v>
       </c>
       <c r="F198" s="11" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="G198" s="31" t="s">
         <v>119</v>
@@ -12791,7 +12785,7 @@
         <v>304</v>
       </c>
       <c r="F199" s="11" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="G199" s="31" t="s">
         <v>48</v>
@@ -12846,7 +12840,7 @@
         <v>229</v>
       </c>
       <c r="F200" s="11" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="G200" s="31" t="s">
         <v>48</v>
@@ -12901,7 +12895,7 @@
         <v>575</v>
       </c>
       <c r="F201" s="11" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="G201" s="31" t="s">
         <v>48</v>
@@ -12934,7 +12928,7 @@
       <c r="T201" s="11"/>
       <c r="U201" s="11"/>
       <c r="V201" s="19" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="W201" s="11"/>
       <c r="X201" s="11"/>
@@ -12958,7 +12952,7 @@
         <v>579</v>
       </c>
       <c r="F202" s="11" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="G202" s="31" t="s">
         <v>48</v>
@@ -12991,7 +12985,7 @@
       <c r="T202" s="11"/>
       <c r="U202" s="11"/>
       <c r="V202" s="11" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="W202" s="11"/>
       <c r="X202" s="11"/>
@@ -13015,7 +13009,7 @@
         <v>581</v>
       </c>
       <c r="F203" s="11" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="G203" s="31" t="s">
         <v>48</v>
@@ -13048,7 +13042,7 @@
       <c r="T203" s="11"/>
       <c r="U203" s="11"/>
       <c r="V203" s="11" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="W203" s="11"/>
       <c r="X203" s="11"/>
@@ -13072,7 +13066,7 @@
         <v>584</v>
       </c>
       <c r="F204" s="11" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="G204" s="31" t="s">
         <v>48</v>
@@ -13105,7 +13099,7 @@
       <c r="T204" s="11"/>
       <c r="U204" s="11"/>
       <c r="V204" s="11" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="W204" s="11"/>
       <c r="X204" s="11"/>
@@ -13129,7 +13123,7 @@
         <v>586</v>
       </c>
       <c r="F205" s="11" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="G205" s="31" t="s">
         <v>48</v>
@@ -13162,7 +13156,7 @@
       <c r="T205" s="11"/>
       <c r="U205" s="11"/>
       <c r="V205" s="11" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="W205" s="11"/>
       <c r="X205" s="11"/>
@@ -13186,7 +13180,7 @@
         <v>590</v>
       </c>
       <c r="F206" s="11" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="G206" s="31" t="s">
         <v>48</v>
@@ -13219,7 +13213,7 @@
       <c r="T206" s="11"/>
       <c r="U206" s="11"/>
       <c r="V206" s="11" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="W206" s="11"/>
       <c r="X206" s="11"/>
@@ -13243,7 +13237,7 @@
         <v>304</v>
       </c>
       <c r="F207" s="11" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="G207" s="31" t="s">
         <v>48</v>
@@ -13276,7 +13270,7 @@
       <c r="T207" s="11"/>
       <c r="U207" s="11"/>
       <c r="V207" s="11" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="W207" s="11"/>
       <c r="X207" s="11"/>
@@ -13300,7 +13294,7 @@
         <v>229</v>
       </c>
       <c r="F208" s="11" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="G208" s="31" t="s">
         <v>48</v>
@@ -13333,7 +13327,7 @@
       <c r="T208" s="11"/>
       <c r="U208" s="11"/>
       <c r="V208" s="11" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="W208" s="11"/>
       <c r="X208" s="11"/>
@@ -13357,7 +13351,7 @@
         <v>575</v>
       </c>
       <c r="F209" s="11" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="G209" s="31" t="s">
         <v>48</v>
@@ -13390,7 +13384,7 @@
       <c r="T209" s="11"/>
       <c r="U209" s="11"/>
       <c r="V209" s="11" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="W209" s="11"/>
       <c r="X209" s="11"/>
@@ -13414,7 +13408,7 @@
         <v>579</v>
       </c>
       <c r="F210" s="11" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="G210" s="31" t="s">
         <v>48</v>
@@ -13447,7 +13441,7 @@
       <c r="T210" s="11"/>
       <c r="U210" s="11"/>
       <c r="V210" s="11" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="W210" s="11"/>
       <c r="X210" s="11"/>
@@ -13471,7 +13465,7 @@
         <v>581</v>
       </c>
       <c r="F211" s="11" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="G211" s="31" t="s">
         <v>48</v>
@@ -13504,7 +13498,7 @@
       <c r="T211" s="11"/>
       <c r="U211" s="11"/>
       <c r="V211" s="11" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="W211" s="11"/>
       <c r="X211" s="11"/>
@@ -13528,7 +13522,7 @@
         <v>584</v>
       </c>
       <c r="F212" s="11" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="G212" s="31" t="s">
         <v>48</v>
@@ -13561,7 +13555,7 @@
       <c r="T212" s="11"/>
       <c r="U212" s="11"/>
       <c r="V212" s="11" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="W212" s="11"/>
       <c r="X212" s="11"/>
@@ -13585,7 +13579,7 @@
         <v>586</v>
       </c>
       <c r="F213" s="11" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="G213" s="31" t="s">
         <v>48</v>
@@ -13618,7 +13612,7 @@
       <c r="T213" s="11"/>
       <c r="U213" s="11"/>
       <c r="V213" s="11" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="W213" s="11"/>
       <c r="X213" s="11"/>
@@ -13642,7 +13636,7 @@
         <v>590</v>
       </c>
       <c r="F214" s="11" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="G214" s="31" t="s">
         <v>48</v>
@@ -13675,7 +13669,7 @@
       <c r="T214" s="11"/>
       <c r="U214" s="11"/>
       <c r="V214" s="11" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="W214" s="11"/>
       <c r="X214" s="11"/>
@@ -15818,8 +15812,8 @@
   </sheetPr>
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -15837,10 +15831,10 @@
         <v>343</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>387</v>
+        <v>708</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>703</v>
+        <v>709</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>345</v>
@@ -15872,9 +15866,7 @@
       <c r="N1" s="1" t="s">
         <v>675</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>387</v>
-      </c>
+      <c r="O1" s="1"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1">
       <c r="A2" s="7" t="s">
@@ -15884,7 +15876,7 @@
         <v>9000</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="D2" s="30">
         <f>2248</f>
@@ -15920,9 +15912,7 @@
       <c r="N2" s="24">
         <v>13025</v>
       </c>
-      <c r="O2" s="11" t="s">
-        <v>419</v>
-      </c>
+      <c r="O2" s="11"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1">
       <c r="A3" s="7" t="s">
@@ -15932,10 +15922,11 @@
         <v>14000</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>676</v>
-      </c>
-      <c r="D3" s="11">
-        <v>1000</v>
+        <v>702</v>
+      </c>
+      <c r="D3" s="30">
+        <f>4588</f>
+        <v>4588</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>355</v>
@@ -15967,9 +15958,7 @@
       <c r="N3" s="24">
         <v>0</v>
       </c>
-      <c r="O3" s="11" t="s">
-        <v>676</v>
-      </c>
+      <c r="O3" s="11"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" customHeight="1">
       <c r="A4" s="7" t="s">
@@ -15978,13 +15967,8 @@
       <c r="B4" s="9">
         <v>12000</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>705</v>
-      </c>
-      <c r="D4" s="30">
-        <f>4588</f>
-        <v>4588</v>
-      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="30"/>
       <c r="I4" s="11" t="s">
         <v>671</v>
       </c>
@@ -15999,9 +15983,7 @@
       </c>
       <c r="M4" s="7"/>
       <c r="N4" s="24"/>
-      <c r="O4" s="11" t="s">
-        <v>677</v>
-      </c>
+      <c r="O4" s="11"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1">
       <c r="A5" s="7" t="s">
@@ -16009,12 +15991,6 @@
       </c>
       <c r="B5" s="9">
         <v>15000</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>706</v>
-      </c>
-      <c r="D5" s="9">
-        <v>0</v>
       </c>
       <c r="I5" s="11" t="s">
         <v>669</v>
@@ -38461,8 +38437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4EC6FB2-1903-0042-ACE8-47D7240CC83A}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -38488,7 +38464,7 @@
         <v>434</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>432</v>
@@ -38499,7 +38475,7 @@
         <v>435</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>432</v>
@@ -38510,7 +38486,7 @@
         <v>436</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>433</v>
@@ -38521,7 +38497,7 @@
         <v>437</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>433</v>
@@ -38532,7 +38508,7 @@
         <v>438</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>433</v>

</xml_diff>